<commit_message>
New Api for Close
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-wf/src/main/resources/plugin/wf/oob/cab/system.workflow.xlsx
+++ b/vertx-pin/zero-wf/src/main/resources/plugin/wf/oob/cab/system.workflow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-wf/src/main/resources/plugin/wf/oob/cab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0ECA0E-39D1-EA49-ADEF-1719B3CFBE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861FB8C2-B850-B348-B551-7D346F53B57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44840" yWindow="-2980" windowWidth="38400" windowHeight="22620" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="168">
   <si>
     <t>key</t>
   </si>
@@ -619,6 +619,28 @@
   </si>
   <si>
     <t>resource.flow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关闭工作流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0c235fe1-24fc-4db1-8be6-a131ff7dfd6c</t>
+  </si>
+  <si>
+    <t>res.up.flow.close</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>849f2149-4abd-4213-9d47-0d1d0b12d051</t>
+  </si>
+  <si>
+    <t>act.up.flow.close</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/up/flow/close</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1266,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6C9C3-8DFE-A442-A082-10767386D931}">
-  <dimension ref="A2:K61"/>
+  <dimension ref="A2:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52:F61"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="21"/>
@@ -1719,7 +1741,7 @@
         <v>64</v>
       </c>
       <c r="B32" s="16" t="str">
-        <f>A50</f>
+        <f>A51</f>
         <v>26cf9250-1238-4c23-9017-0284298412a9</v>
       </c>
       <c r="C32" s="16" t="str">
@@ -1749,7 +1771,7 @@
         <v>71</v>
       </c>
       <c r="B33" s="16" t="str">
-        <f>A51</f>
+        <f>A52</f>
         <v>18aee330-9587-4332-a671-7cab00164036</v>
       </c>
       <c r="C33" s="16" t="str">
@@ -1779,7 +1801,7 @@
         <v>56</v>
       </c>
       <c r="B34" s="16" t="str">
-        <f t="shared" ref="B34:B36" si="0">A52</f>
+        <f t="shared" ref="B34:B36" si="0">A53</f>
         <v>2df451a8-4594-442c-9438-255e40672a0e</v>
       </c>
       <c r="C34" s="16" t="str">
@@ -1866,7 +1888,7 @@
         <v>94</v>
       </c>
       <c r="B37" s="16" t="str">
-        <f t="shared" ref="B37:B38" si="1">A55</f>
+        <f t="shared" ref="B37:B38" si="1">A56</f>
         <v>3ad173b3-7d69-40ec-9089-97f3ac043b6a</v>
       </c>
       <c r="C37" s="16" t="str">
@@ -1926,7 +1948,7 @@
         <v>111</v>
       </c>
       <c r="B39" s="16" t="str">
-        <f t="shared" ref="B39:B40" si="2">A57</f>
+        <f t="shared" ref="B39:B40" si="2">A58</f>
         <v>8ba5f939-3c61-4809-b278-3c0f000bb018</v>
       </c>
       <c r="C39" s="16" t="str">
@@ -1986,7 +2008,7 @@
         <v>126</v>
       </c>
       <c r="B41" s="16" t="str">
-        <f>A59</f>
+        <f>A60</f>
         <v>7093fb25-6740-414a-bdce-70e49f944395</v>
       </c>
       <c r="C41" s="16" t="str">
@@ -2016,7 +2038,7 @@
         <v>142</v>
       </c>
       <c r="B42" s="16" t="str">
-        <f>A60</f>
+        <f>A61</f>
         <v>a9b620eb-795d-4bb6-86c3-5f0491e0a178</v>
       </c>
       <c r="C42" s="16" t="str">
@@ -2043,27 +2065,27 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="10" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B43" s="16" t="str">
-        <f t="shared" ref="B43" si="4">A61</f>
-        <v>449f53a9-12ab-46ab-b4ac-2750b7f59f52</v>
+        <f>A62</f>
+        <v>0c235fe1-24fc-4db1-8be6-a131ff7dfd6c</v>
       </c>
       <c r="C43" s="16" t="str">
         <f>A25</f>
         <v>2e349fcf-5739-4bf5-a24b-e60ff0d4e4b1</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>121</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="H43" s="12">
         <v>8</v>
@@ -2072,24 +2094,45 @@
       <c r="K43" s="14"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="27"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
+      <c r="A44" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="16" t="str">
+        <f t="shared" ref="B44" si="4">A63</f>
+        <v>449f53a9-12ab-46ab-b4ac-2750b7f59f52</v>
+      </c>
+      <c r="C44" s="16" t="str">
+        <f>A25</f>
+        <v>2e349fcf-5739-4bf5-a24b-e60ff0d4e4b1</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="H44" s="12">
+        <v>8</v>
+      </c>
+      <c r="I44" s="12"/>
       <c r="K44" s="14"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="4"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
       <c r="K45" s="14"/>
     </row>
     <row r="46" spans="1:11">
@@ -2102,170 +2145,154 @@
       <c r="K46" s="14"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="4"/>
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C48" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="35"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="35"/>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="5" t="s">
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C49" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F49" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G48" s="18" t="s">
+      <c r="G49" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H49" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="I48" s="18" t="s">
+      <c r="I49" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="7" t="s">
+    <row r="50" spans="1:11">
+      <c r="A50" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B50" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C50" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D50" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E50" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F50" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G50" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="7" t="s">
+      <c r="H50" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I49" s="7" t="s">
+      <c r="I50" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="G50" s="12">
-        <v>1</v>
-      </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="G51" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="10" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G52" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="10" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>132</v>
+        <v>54</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>161</v>
@@ -2278,16 +2305,16 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="10" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>133</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>160</v>
@@ -2303,41 +2330,41 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="10" t="s">
-        <v>92</v>
+        <v>155</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>161</v>
       </c>
       <c r="G55" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>53</v>
@@ -2346,23 +2373,23 @@
         <v>161</v>
       </c>
       <c r="G56" s="12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="10" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E57" s="12" t="s">
         <v>53</v>
@@ -2371,24 +2398,23 @@
         <v>161</v>
       </c>
       <c r="G57" s="12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
-      <c r="K57" s="14"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="10" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>53</v>
@@ -2405,16 +2431,16 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="10" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>53</v>
@@ -2423,23 +2449,24 @@
         <v>161</v>
       </c>
       <c r="G59" s="12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
+      <c r="K59" s="14"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="10" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>53</v>
@@ -2455,16 +2482,16 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="10" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>53</v>
@@ -2477,12 +2504,62 @@
       </c>
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="G62" s="12">
+        <v>8</v>
+      </c>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="G63" s="12">
+        <v>8</v>
+      </c>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>